<commit_message>
completed surprise feature, squashed bugs, final commit hopefully
</commit_message>
<xml_diff>
--- a/platform_compatibility.xlsx
+++ b/platform_compatibility.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msengage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D43D52-816C-422E-A00D-970EF63395F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76C9237-E97A-4371-A02F-221407348D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{730D989E-2977-41A3-97D2-0B4F926BBE0B}"/>
+    <workbookView xWindow="900" yWindow="-108" windowWidth="22248" windowHeight="13176" xr2:uid="{730D989E-2977-41A3-97D2-0B4F926BBE0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,13 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -160,6 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +485,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +563,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>

</xml_diff>